<commit_message>
remove some state transitions
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/state_transition.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/state_transition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frosted-Heart\src\datagen\resources\data\frostedheart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C10EBF-156C-174A-B5C9-DB6DAF87A520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C19E09-516A-4514-92BC-0B05E71D278E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_temperature" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="41">
   <si>
     <t>block</t>
   </si>
@@ -106,18 +106,6 @@
     <t>minecraft:gravel</t>
   </si>
   <si>
-    <t>minecraft:sand</t>
-  </si>
-  <si>
-    <t>minecraft:red_sand</t>
-  </si>
-  <si>
-    <t>frostedheart:bauxite_block</t>
-  </si>
-  <si>
-    <t>frostedheart:kaolin_block</t>
-  </si>
-  <si>
     <t>frostedheart:buried_podzol</t>
   </si>
   <si>
@@ -139,24 +127,9 @@
     <t>frostedheart:gravel_permafrost</t>
   </si>
   <si>
-    <t>frostedheart:sand_permafrost</t>
-  </si>
-  <si>
-    <t>frostedheart:red_sand_permafrost</t>
-  </si>
-  <si>
     <t>frostedheart:clay_permafrost</t>
   </si>
   <si>
-    <t>frostedheart:peat_permafrost</t>
-  </si>
-  <si>
-    <t>frostedheart:bauxite_permafrost</t>
-  </si>
-  <si>
-    <t>frostedheart:kaolin_permafrost</t>
-  </si>
-  <si>
     <t>frostedheart:podzol_permafrost</t>
   </si>
   <si>
@@ -170,16 +143,13 @@
   </si>
   <si>
     <t>minecraft:farmland</t>
-  </si>
-  <si>
-    <t>frostedheart:peat_block</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +172,12 @@
       <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -249,7 +225,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,27 +498,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="166" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L23" sqref="A23:L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.875" customWidth="1"/>
+    <col min="6" max="6" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="21.375" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="9" max="9" width="11.625" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -612,7 +588,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -647,7 +623,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -682,7 +658,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -717,7 +693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -752,7 +728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -787,7 +763,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -822,7 +798,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -857,7 +833,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -892,7 +868,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -906,7 +882,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>24</v>
@@ -927,7 +903,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -941,7 +917,7 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>27</v>
@@ -962,9 +938,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>200</v>
@@ -976,30 +952,30 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <v>-5</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>90</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13">
-        <v>-5</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>90</v>
-      </c>
-      <c r="K13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>200</v>
@@ -1011,30 +987,30 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <v>-5</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>90</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14">
-        <v>-5</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="J14">
-        <v>90</v>
-      </c>
-      <c r="K14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B15" s="2">
         <v>200</v>
@@ -1046,13 +1022,13 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H15">
         <v>-5</v>
@@ -1067,9 +1043,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
         <v>200</v>
@@ -1081,13 +1057,13 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H16">
         <v>-5</v>
@@ -1102,9 +1078,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2">
         <v>200</v>
@@ -1116,30 +1092,30 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17">
+        <v>-5</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>90</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17">
-        <v>-5</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17">
-        <v>90</v>
-      </c>
-      <c r="K17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="B18" s="2">
         <v>200</v>
@@ -1151,13 +1127,13 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H18">
         <v>-5</v>
@@ -1172,9 +1148,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2">
         <v>200</v>
@@ -1185,11 +1161,11 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" t="s">
-        <v>45</v>
+      <c r="E19" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>26</v>
@@ -1207,164 +1183,164 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2">
+        <v>100</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20">
+        <v>-5</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>90</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="2">
-        <v>200</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="B21" s="2">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20">
-        <v>-5</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <v>90</v>
-      </c>
-      <c r="K20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="2" t="s">
+      <c r="F21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21">
+        <v>-5</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>90</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2">
+        <v>100</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22">
+        <v>-5</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>90</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="2">
-        <v>200</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="B23" s="2">
+        <v>100</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21">
-        <v>-5</v>
-      </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>90</v>
-      </c>
-      <c r="K21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="2" t="s">
+      <c r="F23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>-5</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>90</v>
+      </c>
+      <c r="K23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="2">
-        <v>200</v>
-      </c>
-      <c r="C22" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="B24" s="2">
+        <v>100</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22">
-        <v>-5</v>
-      </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22">
-        <v>90</v>
-      </c>
-      <c r="K22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="2">
-        <v>200</v>
-      </c>
-      <c r="C23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23">
-        <v>-5</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="J23">
-        <v>90</v>
-      </c>
-      <c r="K23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="2">
-        <v>200</v>
-      </c>
-      <c r="C24" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>26</v>
@@ -1382,9 +1358,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2">
         <v>100</v>
@@ -1396,12 +1372,12 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H25">
@@ -1417,9 +1393,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2">
         <v>100</v>
@@ -1431,12 +1407,12 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H26">
@@ -1452,9 +1428,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
-        <v>38</v>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B27" s="2">
         <v>100</v>
@@ -1465,14 +1441,14 @@
       <c r="D27" t="s">
         <v>12</v>
       </c>
-      <c r="E27" t="s">
-        <v>38</v>
+      <c r="E27" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H27">
         <v>-5</v>
@@ -1487,27 +1463,27 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" t="s">
-        <v>39</v>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B28" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="G28" t="s">
+        <v>26</v>
       </c>
       <c r="H28">
         <v>-5</v>
@@ -1522,357 +1498,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="2">
-        <v>100</v>
-      </c>
-      <c r="C29" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29">
-        <v>-5</v>
-      </c>
-      <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="J29">
-        <v>90</v>
-      </c>
-      <c r="K29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="2">
-        <v>100</v>
-      </c>
-      <c r="C30" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30">
-        <v>-5</v>
-      </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="J30">
-        <v>90</v>
-      </c>
-      <c r="K30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="2">
-        <v>100</v>
-      </c>
-      <c r="C31" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H31">
-        <v>-5</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31">
-        <v>90</v>
-      </c>
-      <c r="K31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="2">
-        <v>100</v>
-      </c>
-      <c r="C32" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32">
-        <v>-5</v>
-      </c>
-      <c r="I32">
-        <v>2</v>
-      </c>
-      <c r="J32">
-        <v>90</v>
-      </c>
-      <c r="K32">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="2">
-        <v>100</v>
-      </c>
-      <c r="C33" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H33">
-        <v>-5</v>
-      </c>
-      <c r="I33">
-        <v>2</v>
-      </c>
-      <c r="J33">
-        <v>90</v>
-      </c>
-      <c r="K33">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="2">
-        <v>100</v>
-      </c>
-      <c r="C34" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34">
-        <v>-5</v>
-      </c>
-      <c r="I34">
-        <v>2</v>
-      </c>
-      <c r="J34">
-        <v>90</v>
-      </c>
-      <c r="K34">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="2">
-        <v>100</v>
-      </c>
-      <c r="C35" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35">
-        <v>-5</v>
-      </c>
-      <c r="I35">
-        <v>2</v>
-      </c>
-      <c r="J35">
-        <v>90</v>
-      </c>
-      <c r="K35">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="2">
-        <v>100</v>
-      </c>
-      <c r="C36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H36">
-        <v>-5</v>
-      </c>
-      <c r="I36">
-        <v>2</v>
-      </c>
-      <c r="J36">
-        <v>90</v>
-      </c>
-      <c r="K36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="2">
-        <v>100</v>
-      </c>
-      <c r="C37" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H37">
-        <v>-5</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-      <c r="J37">
-        <v>90</v>
-      </c>
-      <c r="K37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C38" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" t="s">
-        <v>26</v>
-      </c>
-      <c r="H38">
-        <v>-5</v>
-      </c>
-      <c r="I38">
-        <v>2</v>
-      </c>
-      <c r="J38">
-        <v>90</v>
-      </c>
-      <c r="K38">
-        <v>100</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Optimize temperature chunk ticks
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/state_transition.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/state_transition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB48DE0-12B7-3C4E-A903-5F8BB921D92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C91162-7B6C-CC41-AB43-85E158F44DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_temperature" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -558,7 +558,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>1</v>
@@ -593,7 +593,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="2">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>1</v>
@@ -698,7 +698,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -733,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>1</v>
@@ -768,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
@@ -803,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="2">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -838,7 +838,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>1</v>
@@ -873,7 +873,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>1</v>
@@ -908,7 +908,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>1</v>
@@ -943,7 +943,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>1</v>
@@ -978,7 +978,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>1</v>
@@ -1048,7 +1048,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
@@ -1083,7 +1083,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -1118,7 +1118,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>1</v>
@@ -1153,7 +1153,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="2">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1" t="b">
         <v>1</v>
@@ -1188,7 +1188,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="b">
         <v>1</v>
@@ -1223,7 +1223,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>1</v>
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>1</v>
@@ -1293,7 +1293,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>1</v>
@@ -1328,7 +1328,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>1</v>
@@ -1363,7 +1363,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>1</v>
@@ -1398,7 +1398,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
@@ -1433,7 +1433,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>1</v>
@@ -1468,7 +1468,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="2">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Increase heat capacity for many blocks - Also dead bush will not cause farmland to disappear now
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/state_transition.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/state_transition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\eclipse-workspace\frostedheart-newdev\src\datagen\resources\data\frostedheart\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyc/Development/FrostedHeart/src/datagen/resources/data/frostedheart/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC33DE1-CEC1-4079-A288-6109B01B25BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A4D03-5A12-EC4C-9E63-4C06A380F175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_temperature" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,7 +272,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -547,25 +547,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="37.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.875" customWidth="1"/>
-    <col min="7" max="7" width="28.375" customWidth="1"/>
-    <col min="8" max="8" width="21.375" customWidth="1"/>
-    <col min="9" max="9" width="11.875" customWidth="1"/>
-    <col min="10" max="10" width="11.625" customWidth="1"/>
-    <col min="11" max="11" width="15.375" customWidth="1"/>
-    <col min="12" max="12" width="14.875" customWidth="1"/>
+    <col min="1" max="2" width="37.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -641,7 +641,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -679,7 +679,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -717,7 +717,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -755,7 +755,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -793,7 +793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -829,7 +829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -865,7 +865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -903,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -941,7 +941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>1</v>
@@ -979,7 +979,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>1</v>
@@ -1017,7 +1017,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1" t="b">
         <v>1</v>
@@ -1053,7 +1053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="b">
         <v>1</v>
@@ -1091,7 +1091,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="b">
         <v>1</v>
@@ -1129,7 +1129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="b">
         <v>1</v>
@@ -1167,7 +1167,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="b">
         <v>1</v>
@@ -1205,7 +1205,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1" t="b">
         <v>1</v>
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1" t="b">
         <v>1</v>
@@ -1281,7 +1281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1" t="b">
         <v>1</v>
@@ -1317,7 +1317,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D30" s="1" t="b">
         <v>0</v>
@@ -1695,7 +1695,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D31" s="1" t="b">
         <v>0</v>
@@ -1731,7 +1731,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D32" s="1" t="b">
         <v>0</v>
@@ -1767,7 +1767,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="2" t="s">
         <v>46</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D33" s="1" t="b">
         <v>0</v>
@@ -1803,7 +1803,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="2" t="s">
         <v>50</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="2" t="s">
         <v>52</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D40" s="1" t="b">
         <v>0</v>
@@ -2067,7 +2067,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>